<commit_message>
& - 20133 от 20.07.2025 https://2eurostore.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Vatican_city/#EURO#Vatican_city#Commemorative#[2004-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Vatican_city/#EURO#Vatican_city#Commemorative#[2004-present]#UNC%varieties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Vatican_city\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C6B04D-597F-4F6A-B461-16C27E596D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B92E8E8-6C20-469A-8A7D-DC804DDEDC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="33150" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -1350,7 +1353,7 @@
       <pane xSplit="9" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1456,7 +1459,7 @@
         <v>45</v>
       </c>
       <c r="G4" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="7" t="str">

</xml_diff>